<commit_message>
Automatische test-sync: 2025-06-24 19:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,8 +720,48 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BTW-nummer toevoegen</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mijn BTW-nummer is niet vermeld op de factuur.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw bericht. Om uw BTW-nummer toe te voegen aan uw factuur, hebben we uw klantgegevens nodig. Kunt u alstublieft uw factuurnummer en het juiste BTW-nummer delen, zodat we dit zo snel mogelijk voor u in orde kunnen maken?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:39:50</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -741,7 +781,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -759,7 +799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -799,6 +839,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -760,8 +760,49 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Herinnering betaling</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ik zie dat ik nog een openstaande betaling heb. Kunt u dit bevestigen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om u beter van dienst te kunnen zijn, heb ik wat aanvullende informatie nodig. Kunt u mij uw klantnummer of factuurnummer doorgeven, zodat ik de openstaande betaling voor u kan controleren?
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam] - E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:42:28</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -781,7 +822,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +863,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -842,7 +883,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,8 +801,49 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Offerte voor 500 stuks</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Graag ontvang ik een offerte voor 500 stuks van product X.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw interesse in product X. Om u een nauwkeurige offerte te kunnen sturen, hebben we wat meer details nodig. Kunt u ons laten weten of u specifieke wensen heeft met betrekking tot de productspecificaties of de leveringsvoorwaarden? Zou u ons ook de gewenste leverdatum kunnen doorgeven?
+Zodra we deze informatie hebben ontvangen, zullen we zo snel mogelijk een offerte voor 500 stuks product X voor u opstellen.
+Met vriendelijke groet,
+[Naam Bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:44:36</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -822,7 +863,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -840,7 +881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -890,6 +931,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -842,8 +842,49 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wat is het verschil tussen product A en product B?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw vraag over de verschillen tussen product A en product B. Product A is een basisversie met standaardfuncties, terwijl product B de uitgebreide versie is met extra functionaliteiten en geavanceerde opties. Als u specifieke vragen heeft over bepaalde functies of prijzen, dan hoor ik graag van u.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:46:43</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -863,7 +904,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -881,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,6 +982,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -883,8 +883,50 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van de beschadiging van het ontvangen product. Om dit probleem snel voor u op te lossen, heb ik wat extra informatie nodig. Kunt u alstublieft een foto van de beschadiging van het product meesturen? Dit zal ons helpen om de situatie beter te begrijpen en een passende oplossing te bieden.
+Ik kijk uit naar uw antwoord.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:48:56</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -904,7 +946,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -945,7 +987,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -955,11 +997,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -925,8 +925,48 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sollicitatie salesfunctie</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hierbij mijn sollicitatie voor de salesfunctie. CV in bijlage.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je interesse in onze openstaande salesfunctie. Ik heb je sollicitatie ontvangen en zal deze zo spoedig mogelijk bekijken. Mocht ik nog aanvullende informatie nodig hebben, dan neem ik contact met je op.
+Met vriendelijke groet,
+[Naam Bedrijf]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:51:02</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -946,7 +986,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -997,7 +1037,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1007,11 +1047,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,8 +965,48 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Order wijzigen</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Kan ik mijn bestelling nog aanpassen?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je bestelling aan te passen, hebben we wat meer informatie nodig. Zou je kunnen aangeven om welke bestelling het gaat en welke specifieke wijzigingen je zou willen doorvoeren? Met deze gegevens kunnen we je verder helpen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:53:09</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -986,7 +1026,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1004,7 +1044,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1074,6 +1114,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1005,8 +1005,53 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Retour is nog niet verwerkt</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ik heb iets teruggestuurd maar hoor niks. Wanneer krijg ik mijn geld terug?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je vraag over de terugbetaling te kunnen beantwoorden, heb ik aanvullende informatie nodig. Zou je mij het volgende kunnen verstrekken:
+- Het ordernummer van de teruggestuurde items.
+- De datum van de retourzending.
+Met deze gegevens kan ik het proces voor de terugbetaling voor je onderzoeken en je verder helpen. 
+Ik kijk uit naar je antwoord,
+Met vriendelijke groet,
+[Jouw Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:55:14</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1026,7 +1071,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1071,7 +1116,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,8 +1050,54 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Retour aanmelden</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ik wil graag een artikel retourneren. Hoe werkt dat?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om een artikel te retourneren, volg je eenvoudig de onderstaande stappen:
+1. Log in op je account op onze website.
+2. Ga naar je bestelgeschiedenis en selecteer de bestelling waarvan je een artikel wilt retourneren.
+3. Klik op de optie 'Retourneren' naast het artikel dat je wilt terugsturen.
+4. Volg de instructies om het retourproces te voltooien en het retourlabel te ontvangen.
+Zodra we het geretourneerde artikel hebben ontvangen en verwerkt, zullen we het aankoopbedrag terugstorten op de oorspronkelijke betaalmethode.
+Mocht je nog vragen hebben of hulp nodig hebben bij het retourneren, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam Bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:57:21</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1071,7 +1117,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1116,7 +1162,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 19:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,8 +1096,50 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Inlogproblemen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ik kan niet meer inloggen op mijn account. Kunnen jullie helpen?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je verder te kunnen helpen met het inlogprobleem, heb ik wat meer informatie nodig. Zou je alsjeblieft je gebruikersnaam willen doorgeven? Hiermee kunnen we het probleem verder onderzoeken en een oplossing bieden.
+Alvast bedankt voor je medewerking.
+Met vriendelijke groet,
+[Naam assistent]
+Nederlandse e-mailassistent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-24 19:59:32</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1117,7 +1159,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1135,7 +1177,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1215,6 +1257,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,8 +1138,40 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kan ik dit product ruilen voor een andere maat?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:01:57</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1159,7 +1191,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1204,7 +1236,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1170,8 +1170,48 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kan mijn wachtwoord niet resetten</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ik krijg geen e-mail bij wachtwoord resetten.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om u beter te kunnen helpen, heb ik wat meer informatie van u nodig. Kunt u mij uw gebruikersnaam of het e-mailadres waarmee u probeert uw wachtwoord te resetten doorgeven? Op die manier kunnen we verder onderzoeken wat er misgaat en u zo snel mogelijk helpen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:04:03</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1191,7 +1231,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1262,17 +1302,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1282,7 +1322,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1292,7 +1332,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1210,8 +1210,48 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Is product Y nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ik wil graag weten of product Y beschikbaar is.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw interesse in product Y. Helaas is product Y op dit moment niet beschikbaar in onze webshop. Wij raden u aan om regelmatig onze website te bezoeken of u in te schrijven voor onze nieuwsbrief om op de hoogte te blijven van nieuwe voorraad en aanbiedingen. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:06:09</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1231,7 +1271,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1302,7 +1342,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1312,17 +1352,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1250,8 +1250,40 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Korting voor wederverkopers?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Biedt u speciale prijzen voor wederverkopers?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:08:18</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1271,7 +1303,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1342,7 +1374,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1352,7 +1384,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1362,11 +1394,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1282,8 +1282,49 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Technische storing</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>De website werkt niet goed. Is hier iets mis mee?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw probleem met de website beter te kunnen onderzoeken, hebben we wat meer informatie nodig. Kunt u specifiek aangeven welke problemen u ervaart bij het gebruik van de website? Krijgt u foutmeldingen te zien, of is er een specifieke pagina die niet laadt? Eventuele details die u kunt verstrekken, zoals de tijd waarop het probleem zich voordeed, zullen ons helpen om het probleem snel op te lossen.
+Met vriendelijke groet,
+[Je naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:10:34</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1303,7 +1344,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1354,17 +1395,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1374,7 +1415,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1384,7 +1425,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1394,7 +1435,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1323,8 +1323,48 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mijn bestelling is incompleet geleverd. Graag hoor ik hoe dit wordt opgelost.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Het spijt me te horen dat uw bestelling incompleet geleverd is. Om dit probleem op te lossen, hebben we wat meer informatie nodig. Kunt u ons uw bestelnummer doorgeven, zodat we kunnen controleren wat er precies misgaan is? Op basis daarvan zullen we zo snel mogelijk een oplossing voor u vinden.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:12:39</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1344,7 +1384,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1449,7 +1489,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1363,8 +1363,48 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw e-mail. Om u zo snel mogelijk te kunnen helpen, hebben we wat extra informatie nodig. Kunt u alstublieft uw klantgegevens (zoals uw naam en e-mailadres) en/of het factuurnummer van uw laatste bestelling doorgeven? Op die manier kunnen we de factuur voor u zo spoedig mogelijk opstellen en toesturen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:14:48</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1384,7 +1424,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1435,7 +1475,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1445,17 +1485,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1403,8 +1403,50 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Status van mijn bestelling</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Wanneer wordt mijn bestelling bezorgd?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw bericht. Om u te kunnen helpen met het checken van de bezorgdatum van uw bestelling, hebben we wat meer informatie nodig. Kunt u ons alstublieft uw bestelnummer doorgeven? Met deze informatie kunnen wij direct voor u nakijken wanneer uw bestelling wordt bezorgd.
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam] 
+Klantenservice Team</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:16:49</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1424,7 +1466,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1495,17 +1537,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1525,7 +1567,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1445,8 +1445,50 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Kan ik dit product ruilen voor een andere maat?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je vraag over het ruilen van het product voor een andere maat te beantwoorden: Ja, dat is mogelijk. We hebben een ruilbeleid waarbij je het product kunt omruilen voor een andere maat, mits het product in de originele staat verkeert en binnen de gestelde termijn wordt geretourneerd. 
+Graag ontvangen wij meer informatie over je bestelling, zoals het ordernummer en de gewenste maat, zodat we je verder kunnen helpen met het proces van ruilen. Aarzel niet om contact met ons op te nemen als je nog vragen hebt.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:44:49</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1466,7 +1508,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1511,7 +1553,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 20:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1487,8 +1487,49 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Productmaat ruilen</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Hoi, ik heb een product ontvangen maar de maat is verkeerd. Mag ik deze omruilen?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Het spijt me te horen dat de maat van het ontvangen product niet klopt. Om je te helpen met de omruiling, hebben we wat extra informatie nodig. Zou je alsjeblieft je bestelnummer en de juiste maat die je wilt ontvangen kunnen doorgeven? Zodra we deze gegevens hebben, zullen we de omruiling in gang zetten.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-24 20:48:12</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1508,7 +1549,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1553,7 +1594,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,8 +1528,91 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wil graag andere maat ontvangen</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Hallo, ik heb het product ontvangen maar de maat is niet goed. Kan ik deze ruilen voor een andere maat?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Vervelend om te horen dat de maat niet juist is. Graag helpen we je verder met het ruilen van het product voor een andere maat. Zou je ons kunnen laten weten welke maat je wilt ontvangen en wat je huidige maat is? Zo kunnen we de ruil snel en correct voor je verwerken.
+We zien je reactie graag tegemoet.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:00:14</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Offerte voor 500 stuks</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Graag ontvang ik een offerte voor 500 stuks van product X.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw interesse in product X. Om u een nauwkeurige offerte te kunnen sturen, hebben we wat aanvullende informatie nodig, zoals eventuele specifieke wensen met betrekking tot het product of de levering. Kunt u ons ook laten weten naar welk adres de producten verzonden moeten worden?
+Zodra we deze gegevens hebben ontvangen, zullen we een offerte voor 500 stuks van product X voor u opstellen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:00:19</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1549,7 +1632,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1594,7 +1677,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -1610,7 +1693,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1620,7 +1703,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1630,17 +1713,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1650,7 +1733,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1611,8 +1611,49 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Kan ik ruilen voor een andere maat?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Ja, het is mogelijk om te ruilen voor een andere maat. Graag ontvangen wij je ordernummer en de maat die je wilt ruilen, zodat we dit verder kunnen afhandelen. Aarzel niet om contact met ons op te nemen als je nog verdere vragen hebt.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:04:41</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1632,7 +1673,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1677,7 +1718,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1652,8 +1652,50 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Productmaat ruilen</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Wil graag andere maat ontvangen
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je beter van dienst te kunnen zijn, vragen we je om wat meer informatie te verstrekken. Zoals de bestelgegevens, zoals het ordernummer en de huidige maat van het product. Op deze manier kunnen we je verzoek zo snel mogelijk verwerken. 
+We zien je reactie graag tegemoet.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:06:06</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1673,7 +1715,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1718,7 +1760,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1694,8 +1694,55 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Omruilen van verkeerd formaat</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Hallo,
+ Ik heb een product ontvangen dat niet de juiste maat is. Is het mogelijk om deze om te ruilen voor de juiste maat? Alvast bedankt!
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. We vinden het vervelend om te horen dat je product niet de juiste maat heeft. We helpen je graag met het omruilen van het product voor de juiste maat.
+Om het omruilproces te starten, hebben we wat meer informatie nodig. Kun je ons alsjeblieft de volgende gegevens sturen:
+- Je ordernummer
+- De naam of beschrijving van het product dat je wilt omruilen
+- De juiste maat van het product
+Zodra we deze informatie hebben ontvangen, zullen we zo snel mogelijk contact met je opnemen om de omruiling in gang te zetten.
+Met vriendelijke groet,
+[E-mailassistent] van [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:15:08</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1715,7 +1762,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1760,7 +1807,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1741,8 +1741,51 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Maat ruilen mogelijk?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Hoi, ik heb per ongeluk de verkeerde maat ontvangen. Is het mogelijk om deze te ruilen voor de juiste maat?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Excuses voor het ongemak dat dit heeft veroorzaakt. Om je te helpen met het omruilen van de verkeerde maat voor de juiste maat, hebben we wat meer informatie nodig. Zou je alsjeblieft je ordernummer en de specifieke maat die je nodig hebt, kunnen doorgeven? Hiermee kunnen we de ruilprocedure voor je in gang zetten.
+Verder, graag ontvangen we ook het artikel dat je hebt ontvangen in de verkeerde maat retour. We voorzien je van de instructies voor het retourneren zodra we bovenstaande informatie hebben ontvangen.
+Bedankt voor je begrip en medewerking. We zien je reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:18:00</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1762,7 +1805,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1807,7 +1850,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1784,8 +1784,49 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Verkeerde maat</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hoi, ik heb een product ontvangen maar de maat is verkeerd. Mag ik deze omruilen?
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Het spijt me te horen dat de maat van het ontvangen product niet klopt. Om je te helpen met de omruiling, hebben we wat extra informatie nodig. Zou je alsjeblieft je bestelnummer en de juiste maat die je wilt ontvangen kunnen doorgeven? Zodra we deze gegevens hebben, zullen we de omruiling in gang zetten.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:26:13</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1805,7 +1846,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1850,7 +1891,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1825,8 +1825,93 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Wat vervelend om te horen dat het product beschadigd is aangekomen. Kunt u ons meer details geven over de schade? Bijvoorbeeld, wat voor product is het en wat voor schade is er precies aan? Eventuele foto's van de schade kunnen ook nuttig zijn.
+Zodra we deze informatie hebben, zullen we ons best doen om een passende oplossing voor u te vinden.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:31:18</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u te kunnen helpen met het versturen van een factuur voor uw laatste bestelling, hebben wij wat extra informatie nodig. Kunt u ons alstublieft de volgende gegevens verstrekken:
+1. Uw bestelnummer
+2. De datum van uw bestelling
+3. Het e-mailadres waarnaar wij de factuur kunnen sturen
+Zodra wij deze gegevens van u hebben ontvangen, zullen wij zo spoedig mogelijk de factuur voor u opstellen en toesturen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:31:20</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1846,7 +1931,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1891,7 +1976,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -1901,7 +1986,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1910,8 +1910,40 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ruilen van product</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Kan ik dit product ruilen voor een andere maat?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:34:51</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1931,7 +1963,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1976,7 +2008,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1942,8 +1942,45 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Order wijzigen</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Kan ik mijn bestelling nog aanpassen?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:36:43</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1963,7 +2000,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2024,11 +2061,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2044,7 +2081,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1963,11 +1963,6 @@
           <t>Bestelling / Levering</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>2025-06-24 21:36:43</t>
@@ -1979,8 +1974,48 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Inlogproblemen</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Ik kan niet meer inloggen op mijn account. Kunnen jullie helpen?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je verder te kunnen helpen met het inlogprobleem, hebben we wat meer informatie nodig. Zou je alsjeblieft je gebruikersnaam en eventuele foutmeldingen die je hebt ontvangen kunnen delen? Op die manier kunnen we het probleem zo snel mogelijk voor je oplossen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:40:16</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2000,7 +2035,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2061,7 +2096,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2071,11 +2106,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2014,8 +2014,52 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u te kunnen helpen met het versturen van een factuur voor uw laatste bestelling, hebben wij wat extra informatie nodig. Kunt u ons alstublieft de volgende gegevens verstrekken:
+1. Uw bestelnummer
+2. De datum van uw bestelling
+3. Het e-mailadres waarnaar wij de factuur kunnen sturen
+Zodra wij deze gegevens van u hebben ontvangen, zullen wij zo spoedig mogelijk de factuur voor u opstellen en toesturen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:43:40</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2035,7 +2079,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2090,7 +2134,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2058,8 +2058,50 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Technische storing</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>De website werkt niet goed. Is hier iets mis mee?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om het probleem beter te kunnen onderzoeken, hebben we meer informatie nodig. Zou je alsjeblieft kunnen aangeven welke specifieke problemen je ervaart wanneer je de website probeert te gebruiken? Bijvoorbeeld, krijg je een foutmelding te zien of lukt het niet om in te loggen? Met deze details kunnen we het probleem gericht aanpakken en een oplossing bieden.
+We horen graag meer van je, zodat we je verder kunnen helpen.
+Met vriendelijke groet,  
+[Tekstschrijver]  
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:47:18</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2079,7 +2121,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2144,7 +2186,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:50:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2100,8 +2100,48 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Is product Y nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ik wil graag weten of product Y beschikbaar is.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je interesse in product Y. Helaas is product Y momenteel niet op voorraad. We verwachten een nieuwe levering binnen twee weken. Mocht je op de hoogte gehouden willen worden wanneer het product weer beschikbaar is, laat het ons dan weten.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:50:17</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2121,7 +2161,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2202,7 +2242,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2212,17 +2252,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 21:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2140,8 +2140,52 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Kunt u mij een factuur sturen voor mijn laatste bestelling?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u te kunnen helpen met het versturen van een factuur voor uw laatste bestelling, hebben wij wat extra informatie nodig. Kunt u ons alstublieft de volgende gegevens verstrekken:
+1. Uw bestelnummer
+2. De datum van uw bestelling
+3. Het e-mailadres waarnaar wij de factuur kunnen sturen
+Zodra wij deze gegevens van u hebben ontvangen, zullen wij zo spoedig mogelijk de factuur voor u opstellen en toesturen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-24 21:53:27</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2161,7 +2205,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2216,7 +2260,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 22:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2184,8 +2184,40 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-24 22:00:20</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2205,7 +2237,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2223,7 +2255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2313,6 +2345,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 22:05:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2216,8 +2216,40 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Herinnering betaling</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Ik zie dat ik nog een openstaande betaling heb. Kunt u dit bevestigen?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-24 22:05:29</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2237,7 +2269,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2292,7 +2324,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 22:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2248,8 +2248,40 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Beschadigd product ontvangen</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Het product dat ik heb ontvangen is beschadigd aangekomen.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-24 22:06:53</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2269,7 +2301,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2384,7 +2416,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-24 22:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-24.xlsx
+++ b/logs/mail_log_2025-06-24.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2280,8 +2280,40 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Mijn bestelling is incompleet geleverd. Graag hoor ik hoe dit wordt opgelost.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-24 22:11:51</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2301,7 +2333,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2376,7 +2408,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>